<commit_message>
Added memory module to simulation
</commit_message>
<xml_diff>
--- a/melody_player/melody.xlsx
+++ b/melody_player/melody.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27960" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27960" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HalfPeriod" sheetId="3" r:id="rId1"/>
@@ -218,9 +218,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -517,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G38"/>
+    <sheetView topLeftCell="A12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -554,7 +555,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>261.63</v>
       </c>
       <c r="C2">
@@ -582,7 +583,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>277.18</v>
       </c>
       <c r="C3">
@@ -610,7 +611,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>293.66000000000003</v>
       </c>
       <c r="C4">
@@ -638,7 +639,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>311.13</v>
       </c>
       <c r="C5">
@@ -666,7 +667,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>329.63</v>
       </c>
       <c r="C6">
@@ -694,7 +695,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>349.23</v>
       </c>
       <c r="C7">
@@ -722,7 +723,7 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>369.99</v>
       </c>
       <c r="C8">
@@ -750,7 +751,7 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>392</v>
       </c>
       <c r="C9">
@@ -778,7 +779,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>415.3</v>
       </c>
       <c r="C10">
@@ -806,7 +807,7 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>440</v>
       </c>
       <c r="C11">
@@ -834,7 +835,7 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>466.16</v>
       </c>
       <c r="C12">
@@ -862,7 +863,7 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>493.88</v>
       </c>
       <c r="C13">
@@ -890,7 +891,7 @@
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>523.25</v>
       </c>
       <c r="C14">
@@ -918,7 +919,7 @@
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>554.37</v>
       </c>
       <c r="C15">
@@ -946,7 +947,7 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>587.33000000000004</v>
       </c>
       <c r="C16">
@@ -974,7 +975,7 @@
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>622.25</v>
       </c>
       <c r="C17">
@@ -1002,7 +1003,7 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>659.26</v>
       </c>
       <c r="C18">
@@ -1030,7 +1031,7 @@
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>698.46</v>
       </c>
       <c r="C19">
@@ -1058,7 +1059,7 @@
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>739.99</v>
       </c>
       <c r="C20">
@@ -1086,7 +1087,7 @@
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>783.99</v>
       </c>
       <c r="C21">
@@ -1114,7 +1115,7 @@
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>830.61</v>
       </c>
       <c r="C22">
@@ -1142,7 +1143,7 @@
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>880</v>
       </c>
       <c r="C23">
@@ -1170,7 +1171,7 @@
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>932.33</v>
       </c>
       <c r="C24">
@@ -1198,7 +1199,7 @@
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>987.77</v>
       </c>
       <c r="C25">
@@ -1226,7 +1227,7 @@
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>1046.5</v>
       </c>
       <c r="C26">
@@ -1254,7 +1255,7 @@
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>1108.73</v>
       </c>
       <c r="C27">
@@ -1282,7 +1283,7 @@
       <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>1174.6600000000001</v>
       </c>
       <c r="C28">
@@ -1310,7 +1311,7 @@
       <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>1244.51</v>
       </c>
       <c r="C29">
@@ -1338,7 +1339,7 @@
       <c r="A30" t="s">
         <v>5</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>1318.51</v>
       </c>
       <c r="C30">
@@ -1366,7 +1367,7 @@
       <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>1396.91</v>
       </c>
       <c r="C31">
@@ -1394,7 +1395,7 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>1479.98</v>
       </c>
       <c r="C32">
@@ -1422,7 +1423,7 @@
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>1567.98</v>
       </c>
       <c r="C33">
@@ -1450,7 +1451,7 @@
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>1661.22</v>
       </c>
       <c r="C34">
@@ -1478,7 +1479,7 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>1760</v>
       </c>
       <c r="C35">
@@ -1506,7 +1507,7 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>1864.66</v>
       </c>
       <c r="C36">
@@ -1534,7 +1535,7 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>1975.53</v>
       </c>
       <c r="C37">
@@ -1589,15 +1590,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1623,16 +1625,15 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>41</v>
+      <c r="A2" s="1">
+        <v>64</v>
       </c>
       <c r="B2">
-        <f>B3*1.5</f>
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C2" t="str">
         <f>DEC2HEX(B2,4)</f>
-        <v>0030</v>
+        <v>0020</v>
       </c>
       <c r="D2" t="str">
         <f>MID(C2,1,2)</f>
@@ -1640,23 +1641,24 @@
       </c>
       <c r="E2" t="str">
         <f>MID(C2,3,2)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G2" t="str">
-        <f>$A$18&amp;A2&amp;$A$18&amp;": "&amp;$A$18&amp;C2&amp;$A$18&amp;","</f>
-        <v>"64.": "0030",</v>
+        <f>$A$17&amp;A2&amp;$A$17&amp;": "&amp;$A$17&amp;C2&amp;$A$17&amp;","</f>
+        <v>"64": "0020",</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>64</v>
+      <c r="A3" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B3">
-        <v>32</v>
+        <f>B2*1.5</f>
+        <v>48</v>
       </c>
       <c r="C3" t="str">
         <f>DEC2HEX(B3,4)</f>
-        <v>0020</v>
+        <v>0030</v>
       </c>
       <c r="D3" t="str">
         <f>MID(C3,1,2)</f>
@@ -1664,60 +1666,60 @@
       </c>
       <c r="E3" t="str">
         <f>MID(C3,3,2)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G15" si="0">$A$18&amp;A3&amp;$A$18&amp;": "&amp;$A$18&amp;C3&amp;$A$18&amp;","</f>
-        <v>"64": "0020",</v>
+        <f>$A$17&amp;A3&amp;$A$17&amp;": "&amp;$A$17&amp;C3&amp;$A$17&amp;","</f>
+        <v>"64.": "0030",</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>64</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C14" si="0">DEC2HEX(B4,4)</f>
+        <v>0040</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D14" si="1">MID(C4,1,2)</f>
+        <v>00</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" ref="E4:E14" si="2">MID(C4,3,2)</f>
+        <v>40</v>
+      </c>
+      <c r="G4" t="str">
+        <f>$A$17&amp;A4&amp;$A$17&amp;": "&amp;$A$17&amp;C4&amp;$A$17&amp;","</f>
+        <v>"32": "0040",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4">
-        <f>B5*1.5</f>
+      <c r="B5">
+        <f>B4*1.5</f>
         <v>96</v>
       </c>
-      <c r="C4" t="str">
-        <f>DEC2HEX(B4,4)</f>
+      <c r="C5" t="str">
+        <f>DEC2HEX(B5,4)</f>
         <v>0060</v>
       </c>
-      <c r="D4" t="str">
-        <f>MID(C4,1,2)</f>
+      <c r="D5" t="str">
+        <f>MID(C5,1,2)</f>
         <v>00</v>
       </c>
-      <c r="E4" t="str">
-        <f>MID(C4,3,2)</f>
+      <c r="E5" t="str">
+        <f>MID(C5,3,2)</f>
         <v>60</v>
       </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
+      <c r="G5" t="str">
+        <f>$A$17&amp;A5&amp;$A$17&amp;": "&amp;$A$17&amp;C5&amp;$A$17&amp;","</f>
         <v>"32.": "0060",</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>32</v>
-      </c>
-      <c r="B5">
-        <v>64</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" ref="C5:C15" si="1">DEC2HEX(B5,4)</f>
-        <v>0040</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" ref="D5:D15" si="2">MID(C5,1,2)</f>
-        <v>00</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" ref="E5:E15" si="3">MID(C5,3,2)</f>
-        <v>40</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>"32": "0040",</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1740,7 +1742,7 @@
         <v>BB</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
+        <f>$A$17&amp;A6&amp;$A$17&amp;": "&amp;$A$17&amp;C6&amp;$A$17&amp;","</f>
         <v>"16.": "00BB",</v>
       </c>
     </row>
@@ -1752,224 +1754,225 @@
         <v>125</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>007D</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>00</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7D</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
+        <f>$A$17&amp;A7&amp;$A$17&amp;": "&amp;$A$17&amp;C7&amp;$A$17&amp;","</f>
         <v>"16": "007D",</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>250</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>00FA</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>FA</v>
+      </c>
+      <c r="G8" t="str">
+        <f>$A$17&amp;A8&amp;$A$17&amp;": "&amp;$A$17&amp;C8&amp;$A$17&amp;","</f>
+        <v>"8": "00FA",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B8">
-        <f>B9*1.5</f>
+      <c r="B9">
+        <f>B8*1.5</f>
         <v>375</v>
       </c>
-      <c r="C8" t="str">
-        <f>DEC2HEX(B8,4)</f>
+      <c r="C9" t="str">
+        <f>DEC2HEX(B9,4)</f>
         <v>0177</v>
       </c>
-      <c r="D8" t="str">
-        <f>MID(C8,1,2)</f>
+      <c r="D9" t="str">
+        <f>MID(C9,1,2)</f>
         <v>01</v>
       </c>
-      <c r="E8" t="str">
-        <f>MID(C8,3,2)</f>
+      <c r="E9" t="str">
+        <f>MID(C9,3,2)</f>
         <v>77</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
+      <c r="G9" t="str">
+        <f>$A$17&amp;A9&amp;$A$17&amp;": "&amp;$A$17&amp;C9&amp;$A$17&amp;","</f>
         <v>"8.": "0177",</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>250</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>00FA</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="2"/>
-        <v>00</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="3"/>
-        <v>FA</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>"8": "00FA",</v>
-      </c>
-    </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>500</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>01F4</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>F4</v>
+      </c>
+      <c r="G10" t="str">
+        <f>$A$17&amp;A10&amp;$A$17&amp;": "&amp;$A$17&amp;C10&amp;$A$17&amp;","</f>
+        <v>"4": "01F4",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10">
-        <f>B11*1.5</f>
+      <c r="B11">
+        <f>B10*1.5</f>
         <v>750</v>
       </c>
-      <c r="C10" t="str">
-        <f>DEC2HEX(B10,4)</f>
+      <c r="C11" t="str">
+        <f>DEC2HEX(B11,4)</f>
         <v>02EE</v>
       </c>
-      <c r="D10" t="str">
-        <f>MID(C10,1,2)</f>
+      <c r="D11" t="str">
+        <f>MID(C11,1,2)</f>
         <v>02</v>
       </c>
-      <c r="E10" t="str">
-        <f>MID(C10,3,2)</f>
+      <c r="E11" t="str">
+        <f>MID(C11,3,2)</f>
         <v>EE</v>
       </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
+      <c r="G11" t="str">
+        <f>$A$17&amp;A11&amp;$A$17&amp;": "&amp;$A$17&amp;C11&amp;$A$17&amp;","</f>
         <v>"4.": "02EE",</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>500</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>01F4</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="2"/>
-        <v>01</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="3"/>
-        <v>F4</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>"4": "01F4",</v>
-      </c>
-    </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>03E8</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>03</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>E8</v>
+      </c>
+      <c r="G12" t="str">
+        <f>$A$17&amp;A12&amp;$A$17&amp;": "&amp;$A$17&amp;C12&amp;$A$17&amp;","</f>
+        <v>"2": "03E8",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B12">
-        <f>B13*1.5</f>
+      <c r="B13">
+        <f>B12*1.5</f>
         <v>1500</v>
       </c>
-      <c r="C12" t="str">
-        <f>DEC2HEX(B12,4)</f>
+      <c r="C13" t="str">
+        <f>DEC2HEX(B13,4)</f>
         <v>05DC</v>
       </c>
-      <c r="D12" t="str">
-        <f>MID(C12,1,2)</f>
+      <c r="D13" t="str">
+        <f>MID(C13,1,2)</f>
         <v>05</v>
       </c>
-      <c r="E12" t="str">
-        <f>MID(C12,3,2)</f>
+      <c r="E13" t="str">
+        <f>MID(C13,3,2)</f>
         <v>DC</v>
       </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
+      <c r="G13" t="str">
+        <f>$A$17&amp;A13&amp;$A$17&amp;": "&amp;$A$17&amp;C13&amp;$A$17&amp;","</f>
         <v>"2.": "05DC",</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>1000</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>03E8</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="2"/>
-        <v>03</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="3"/>
-        <v>E8</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>"2": "03E8",</v>
-      </c>
-    </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2000</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>07D0</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>07</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>D0</v>
+      </c>
+      <c r="G14" t="str">
+        <f>$A$17&amp;A14&amp;$A$17&amp;": "&amp;$A$17&amp;C14&amp;$A$17&amp;","</f>
+        <v>"1": "07D0",</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14">
-        <f>B15*1.5</f>
+      <c r="B15">
+        <f>B14*1.5</f>
         <v>3000</v>
       </c>
-      <c r="C14" t="str">
-        <f>DEC2HEX(B14,4)</f>
+      <c r="C15" t="str">
+        <f>DEC2HEX(B15,4)</f>
         <v>0BB8</v>
       </c>
-      <c r="D14" t="str">
-        <f>MID(C14,1,2)</f>
+      <c r="D15" t="str">
+        <f>MID(C15,1,2)</f>
         <v>0B</v>
       </c>
-      <c r="E14" t="str">
-        <f>MID(C14,3,2)</f>
+      <c r="E15" t="str">
+        <f>MID(C15,3,2)</f>
         <v>B8</v>
       </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
+      <c r="G15" t="str">
+        <f>$A$17&amp;A15&amp;$A$17&amp;": "&amp;$A$17&amp;C15&amp;$A$17&amp;","</f>
         <v>"1.": "0BB8",</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>2000</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v>07D0</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="2"/>
-        <v>07</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="3"/>
-        <v>D0</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v>"1": "07D0",</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>